<commit_message>
add date to distri list
</commit_message>
<xml_diff>
--- a/files/07_11_2022.xlsx
+++ b/files/07_11_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgand\go\src\github.com\gandharvas\crs\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A9C0AA-529E-4999-8E72-BDCEA2B788F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38D703F-01DC-428A-B0D0-550A4D2615B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{667EEE24-0357-4A74-9789-2CF5245EFEB5}"/>
   </bookViews>
@@ -91,9 +91,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,7 +123,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>